<commit_message>
format jam 24 jam
</commit_message>
<xml_diff>
--- a/media/download/barang/2d4190ef-e679-44e5-8fde-909e50899242.xlsx
+++ b/media/download/barang/2d4190ef-e679-44e5-8fde-909e50899242.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>barcode</t>
   </si>
@@ -473,8 +473,8 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
+      <c r="D2">
+        <v>10</v>
       </c>
       <c r="E2">
         <v>15000</v>
@@ -496,8 +496,8 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>20000</v>
@@ -519,8 +519,8 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
         <v>25000</v>
@@ -542,8 +542,8 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
         <v>20000</v>
@@ -565,8 +565,8 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>20000</v>
@@ -588,8 +588,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7">
         <v>20000</v>

</xml_diff>